<commit_message>
Feat functions error handler
</commit_message>
<xml_diff>
--- a/excel-files/examples/img-download-template.xlsx
+++ b/excel-files/examples/img-download-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geffe\Desktop\codigo\vtex-wizard\excel-files\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403536DF-9D4E-4D7C-8D5B-759361C037CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDA4A8D-8D27-4639-A643-9807CE741122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8B9850FB-3DED-4EEE-9074-541AEF78CC97}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>SKU</t>
   </si>
@@ -54,19 +54,13 @@
   </si>
   <si>
     <t>M-P6-C33</t>
-  </si>
-  <si>
-    <t>Example of a product with more than one image</t>
-  </si>
-  <si>
-    <t>Example of a product with a single image</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,18 +74,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -121,12 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,18 +448,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1A4827-8481-4A28-9482-4A98454EB8C2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C1" sqref="C1:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="3" max="3" width="37.21875" customWidth="1"/>
+    <col min="3" max="3" width="37.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,26 +467,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>